<commit_message>
develop base summary table builder
</commit_message>
<xml_diff>
--- a/AppData/report.xlsx
+++ b/AppData/report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="106">
   <si>
     <t xml:space="preserve">Результаты итоговой аттестации (отметка, № протокола, дата)</t>
   </si>
@@ -159,220 +159,223 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">Very very subject 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very very subject 19</t>
+    <t xml:space="preserve">Компьютерное проектирование и языки программирования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тестирование программного обеспечения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Программное обеспечение обработки графической информации</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бухгалтерский учет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Физическая культура и здоровье</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Программное средства создания интернет приложений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основы предпринимальской деятельности и управления проектами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Программирование мобильных приложений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Учебная практика по разработке и сопровождению ПО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Учебная практика по веб программированию</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Технологическая практика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Преддипломная практика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диплом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Охрана труда</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основы социально гуманитарных наук</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основы алгаритмизации и программирования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Теория вероятностей и математическая статистика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Арифметико-логические основы вычислительной техники</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Инструментальное программное обеспечение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Техника коммуникаций и основы командообразования</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Иностранный язык (профессион лексика)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Компьютерные сети</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 0</t>
+    <t xml:space="preserve">Бондарук Э. А.</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 1</t>
+    <t xml:space="preserve">Голёта А. А.</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 2</t>
+    <t xml:space="preserve">Грищук С. М.</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 3</t>
+    <t xml:space="preserve">Данченко К. И.</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 4</t>
+    <t xml:space="preserve">Долмат Д. В.</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 5</t>
+    <t xml:space="preserve">Домащук А. С.</t>
   </si>
   <si>
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 6</t>
+    <t xml:space="preserve">Заец Ю. А.</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 7</t>
+    <t xml:space="preserve">Козик Д. В.</t>
   </si>
   <si>
     <t xml:space="preserve">9</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 8</t>
+    <t xml:space="preserve">Концевич В. В.</t>
   </si>
   <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 9</t>
+    <t xml:space="preserve">Корневич М. А.</t>
   </si>
   <si>
     <t xml:space="preserve">11</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 10</t>
+    <t xml:space="preserve">Кушнерук Е. М.</t>
   </si>
   <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 11</t>
+    <t xml:space="preserve">Логинов Д. А.</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 12</t>
+    <t xml:space="preserve">Матюхов Д. И.</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 13</t>
+    <t xml:space="preserve">Невдах В. Э.</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 14</t>
+    <t xml:space="preserve">Пупчик Н. А.</t>
   </si>
   <si>
     <t xml:space="preserve">16</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 15</t>
+    <t xml:space="preserve">Рудаков Н. А.</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 16</t>
+    <t xml:space="preserve">Сачковская Н. В.</t>
   </si>
   <si>
     <t xml:space="preserve">18</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 17</t>
+    <t xml:space="preserve">Слаута А. Е.</t>
   </si>
   <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 18</t>
+    <t xml:space="preserve">Федчук Д. П.</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
   </si>
   <si>
-    <t xml:space="preserve">Student 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Зач</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Осв</t>
+    <t xml:space="preserve">Филиппов И. А.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фицнер А. В.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хаванский С. М.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чечун М. В.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шостак А. И.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шпак М. Г.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">err</t>
   </si>
   <si>
     <t xml:space="preserve">Главное управление по образованию Брестского облисполкома</t>
@@ -516,20 +519,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -568,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -634,38 +629,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1021,7 +984,7 @@
   <dimension ref="A1:AP8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="AS8" sqref="AS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +999,7 @@
   <sheetData>
     <row r="1" spans="1:42" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
@@ -1120,7 +1083,7 @@
     </row>
     <row r="3" spans="1:42" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -1204,7 +1167,7 @@
     </row>
     <row r="5" spans="1:42" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -1256,67 +1219,77 @@
         <v>30</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="J7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="Q7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="S7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="T7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="U7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="V7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="W7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="U7" s="7" t="s">
+      <c r="X7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="V7" s="7" t="s">
+      <c r="Y7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
+      <c r="Z7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -1337,76 +1310,86 @@
     </row>
     <row r="8" spans="1:42" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
+        <v>102</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA8" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="AB8" s="9"/>
       <c r="AC8" s="9"/>
       <c r="AD8" s="9"/>
@@ -1425,85 +1408,85 @@
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X9" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y9" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z9" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA9" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>29</v>
@@ -1553,85 +1536,85 @@
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z10" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA10" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>29</v>
@@ -1681,85 +1664,85 @@
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y11" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z11" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA11" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB11" s="9" t="s">
         <v>29</v>
@@ -1809,85 +1792,85 @@
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T12" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V12" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X12" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z12" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA12" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB12" s="9" t="s">
         <v>29</v>
@@ -1937,85 +1920,85 @@
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="T13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA13" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB13" s="9" t="s">
         <v>29</v>
@@ -2065,85 +2048,85 @@
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="V14" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y14" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z14" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA14" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB14" s="9" t="s">
         <v>29</v>
@@ -2193,85 +2176,85 @@
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="V15" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y15" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z15" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA15" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB15" s="9" t="s">
         <v>29</v>
@@ -2321,85 +2304,85 @@
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R16" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T16" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U16" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V16" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W16" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y16" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z16" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA16" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB16" s="9" t="s">
         <v>29</v>
@@ -2449,85 +2432,85 @@
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S17" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T17" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U17" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V17" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X17" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y17" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z17" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA17" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB17" s="9" t="s">
         <v>29</v>
@@ -2577,85 +2560,85 @@
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S18" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T18" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U18" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V18" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W18" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X18" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y18" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z18" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA18" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB18" s="9" t="s">
         <v>29</v>
@@ -2705,85 +2688,85 @@
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S19" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T19" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U19" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V19" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X19" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y19" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z19" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA19" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB19" s="9" t="s">
         <v>29</v>
@@ -2833,85 +2816,85 @@
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="38" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S20" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T20" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V20" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W20" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X20" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y20" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z20" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA20" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB20" s="9" t="s">
         <v>29</v>
@@ -2961,85 +2944,85 @@
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="U21" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V21" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="X21" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Y21" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="Z21" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AA21" s="9" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="AB21" s="9" t="s">
         <v>29</v>
@@ -3089,129 +3072,1409 @@
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP22" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP23" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA24" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP26" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N22" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="C27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP27" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="C28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP28" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="C29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA29" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="T22" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="U22" s="9" t="s">
+      <c r="C30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="V22" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="W22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP22" s="3" t="s">
+      <c r="C31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA31" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP31" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="R32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="T32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="X32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3238,35 +4501,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="6.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="14" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="14" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" style="14" customWidth="1"/>
-    <col min="19" max="19" width="6.5703125" style="14" customWidth="1"/>
-    <col min="20" max="20" width="6.5703125" style="14" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="14" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" style="14" customWidth="1"/>
-    <col min="23" max="23" width="6.5703125" style="14" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" style="14" customWidth="1"/>
-    <col min="25" max="25" width="6.5703125" style="14" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" style="14" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" style="14" customWidth="1"/>
-    <col min="27" max="27" width="6.5703125" style="14" customWidth="1"/>
     <col min="1" max="1" width="4.42578125" style="14" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" style="14" customWidth="1"/>
-    <col min="28" max="28" width="6.5703125" style="14" customWidth="1"/>
+    <col min="3" max="29" width="6.5703125" style="14" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -3274,81 +4511,26 @@
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" s="24" t="s">
-        <v>29</v>
-      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
     </row>
     <row r="2" spans="1:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:23" ht="186.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3358,544 +4540,7 @@
       <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="C3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.2362204724409449" right="0.2362204724409449" top="0.2362204724409449" bottom="0.2362204724409449" header="0" footer="0"/>

</xml_diff>